<commit_message>
UPdated venn diagram and heatmap
</commit_message>
<xml_diff>
--- a/analysis/UniprotAnnotations_NetworkAnalysis/General_proteome_characterization/PreliminaryProteomeCharacterization.xlsx
+++ b/analysis/UniprotAnnotations_NetworkAnalysis/General_proteome_characterization/PreliminaryProteomeCharacterization.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/OysterSeedProject/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shelly/Documents/GitHub/OysterSeedProject/analysis/UniprotAnnotations_NetworkAnalysis/General_proteome_characterization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D2333B-487C-E84E-953C-E8670AD16CA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1B081E-1FFF-0248-89FB-29EF3EE07A85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3140" yWindow="1160" windowWidth="21060" windowHeight="11020" xr2:uid="{E4D4141F-9E7A-AF49-93CF-6C29E7FAD514}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -560,8 +560,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.208223972003499E-3"/>
-              <c:y val="0.282561606882473"/>
+              <c:x val="1.6097112860892389E-2"/>
+              <c:y val="0.14367271799358414"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1609,7 +1609,7 @@
   <dimension ref="B1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>